<commit_message>
Inserindo Massa de Dados Sena Biblio
</commit_message>
<xml_diff>
--- a/starterDB/NN.xlsx
+++ b/starterDB/NN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arley.saugusto\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arley.saugusto\Documents\REPOS_TURMAS\SenaBiblio-TII01\starterDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53C58887-089D-4EEF-AB4B-5B6018BFC179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F53075E-67FF-432E-948C-F82B3AF18419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{62286D9B-392B-4B90-928F-8A95DF34992E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Conta</t>
   </si>
@@ -126,10 +126,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -468,26 +468,25 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I10" sqref="I10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -524,11 +523,11 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -569,16 +568,16 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
       <c r="I9">
         <v>2</v>
       </c>
@@ -591,10 +590,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -603,9 +602,6 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
         <v>4</v>
       </c>
       <c r="I10">
@@ -619,10 +615,7 @@
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="1">
         <v>10000</v>
       </c>
     </row>
@@ -630,10 +623,7 @@
       <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="1">
         <v>900000</v>
       </c>
     </row>
@@ -641,15 +631,12 @@
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
+      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>